<commit_message>
updated missing MulchGeo tables in excel input files
</commit_message>
<xml_diff>
--- a/Example input/AgmipET2/AGMIPET2Sim.xlsx
+++ b/Example input/AgmipET2/AGMIPET2Sim.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25128"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65DADB0F-1894-4706-AF22-7A65514188B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E8004F0-16F2-44C2-9DD5-44A5D257595C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20232" yWindow="1404" windowWidth="17856" windowHeight="9912" tabRatio="848" firstSheet="4" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4356" yWindow="2940" windowWidth="17856" windowHeight="9912" tabRatio="848" firstSheet="5" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Description" sheetId="16" r:id="rId1"/>
@@ -24,6 +24,7 @@
     <sheet name="Variety" sheetId="10" r:id="rId14"/>
     <sheet name="Weather" sheetId="7" r:id="rId15"/>
     <sheet name="MulchDecomp" sheetId="19" r:id="rId16"/>
+    <sheet name="MulchGeo" sheetId="20" r:id="rId17"/>
   </sheets>
   <definedNames>
     <definedName name="Description">Description!$A$1:$R$11</definedName>
@@ -53,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1559" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1575" uniqueCount="296">
   <si>
     <t>Date</t>
   </si>
@@ -900,6 +901,48 @@
   <si>
     <t>LIGN Decomp</t>
   </si>
+  <si>
+    <t>Min_Hori_Size</t>
+  </si>
+  <si>
+    <t>Diffusion_Restriction</t>
+  </si>
+  <si>
+    <t>LongWaveRadiationCtrl</t>
+  </si>
+  <si>
+    <t>Decomposition_ctrl</t>
+  </si>
+  <si>
+    <t>DeltaRshort</t>
+  </si>
+  <si>
+    <t>DeltaRlong</t>
+  </si>
+  <si>
+    <t>Omega</t>
+  </si>
+  <si>
+    <t>epsilon_mulch</t>
+  </si>
+  <si>
+    <t>alpha_mulch</t>
+  </si>
+  <si>
+    <t>MaxStep in Picard Iteration</t>
+  </si>
+  <si>
+    <t>Tolerance_head</t>
+  </si>
+  <si>
+    <t>rho_mulch</t>
+  </si>
+  <si>
+    <t>pore_space</t>
+  </si>
+  <si>
+    <t>MaxPondingDepth</t>
+  </si>
 </sst>
 </file>
 
@@ -29903,9 +29946,10 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{412C87A0-8875-45CB-B134-6AC3431B7460}">
+  <sheetPr codeName="Sheet16"/>
   <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -30000,6 +30044,116 @@
       </c>
       <c r="L2" s="21">
         <v>2.2800000000000001E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC333C73-500D-4383-8BD8-038545C47371}">
+  <sheetPr codeName="Sheet17"/>
+  <dimension ref="A1:O2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>282</v>
+      </c>
+      <c r="C1" t="s">
+        <v>283</v>
+      </c>
+      <c r="D1" t="s">
+        <v>284</v>
+      </c>
+      <c r="E1" t="s">
+        <v>285</v>
+      </c>
+      <c r="F1" t="s">
+        <v>286</v>
+      </c>
+      <c r="G1" t="s">
+        <v>287</v>
+      </c>
+      <c r="H1" t="s">
+        <v>288</v>
+      </c>
+      <c r="I1" t="s">
+        <v>289</v>
+      </c>
+      <c r="J1" t="s">
+        <v>290</v>
+      </c>
+      <c r="K1" t="s">
+        <v>291</v>
+      </c>
+      <c r="L1" t="s">
+        <v>292</v>
+      </c>
+      <c r="M1" t="s">
+        <v>293</v>
+      </c>
+      <c r="N1" t="s">
+        <v>294</v>
+      </c>
+      <c r="O1" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>269</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>0.3</v>
+      </c>
+      <c r="G2">
+        <v>0.3</v>
+      </c>
+      <c r="H2">
+        <v>0.6</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>0.3</v>
+      </c>
+      <c r="K2">
+        <v>10</v>
+      </c>
+      <c r="L2">
+        <v>0.01</v>
+      </c>
+      <c r="M2">
+        <v>400000</v>
+      </c>
+      <c r="N2">
+        <v>0.8</v>
+      </c>
+      <c r="O2">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated excel input files for revised units and ponded irrigation. updated help file
</commit_message>
<xml_diff>
--- a/Example input/AgmipET2/AGMIPET2Sim.xlsx
+++ b/Example input/AgmipET2/AGMIPET2Sim.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27830"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8012406B-09AC-42EA-BADC-EA1242104278}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{517AD039-48EF-4106-A181-C8D34BD7EAAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="25920" windowHeight="13425" tabRatio="848" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5415" yWindow="2385" windowWidth="21600" windowHeight="11295" tabRatio="848" firstSheet="6" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Description" sheetId="16" r:id="rId1"/>
@@ -165,6 +165,40 @@
           </rPr>
           <t xml:space="preserve">
 hour of day 0-23</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Author</author>
+  </authors>
+  <commentList>
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{45E69C53-1464-4411-BF4F-118A2EAB4DAB}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+ug/cm3 for all C and N fractions</t>
         </r>
       </text>
     </comment>
@@ -1188,7 +1222,7 @@
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="h:mm;@"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1248,6 +1282,19 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1352,7 +1399,8 @@
       </fill>
     </dxf>
   </dxfs>
-  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9">
+  <tableStyles count="2" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9">
+    <tableStyle name="Invisible" pivot="0" table="0" count="0" xr9:uid="{0D770FF7-E571-4A91-90A3-D60CA9D88488}"/>
     <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
@@ -4644,12 +4692,12 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <sheetPr codeName="Sheet9"/>
   <dimension ref="A1:AT213"/>
   <sheetViews>
     <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="Q2" sqref="Q2:Q213"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -34483,6 +34531,7 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter alignWithMargins="0"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -36522,8 +36571,8 @@
   <sheetPr codeName="Sheet20"/>
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -36584,7 +36633,7 @@
         <v>-100000</v>
       </c>
       <c r="F2" s="4">
-        <v>10000000000</v>
+        <v>1E-3</v>
       </c>
       <c r="G2">
         <v>0.02</v>
@@ -41414,7 +41463,7 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:K212"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J2" sqref="J2:K9"/>
     </sheetView>
   </sheetViews>

</xml_diff>